<commit_message>
Working app, need a lot of improvement but works, adde back admin check and fixed goin in and out of activirty display
</commit_message>
<xml_diff>
--- a/backend/reports/scanned_boxes_report.xlsx
+++ b/backend/reports/scanned_boxes_report.xlsx
@@ -597,11 +597,19 @@
       <c r="C8" t="n">
         <v>300</v>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Milica1</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2025-04-06 13:05:31</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
     </row>
@@ -617,11 +625,19 @@
       <c r="C9" t="n">
         <v>300</v>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Milica1</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2025-04-06 13:05:32</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added email sending functionality
</commit_message>
<xml_diff>
--- a/backend/reports/scanned_boxes_report.xlsx
+++ b/backend/reports/scanned_boxes_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,19 +477,11 @@
       <c r="C2" t="n">
         <v>300</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Milica1</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2025-04-06 22:18:49</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
     </row>
@@ -545,11 +537,19 @@
       <c r="C5" t="n">
         <v>300</v>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Milica1</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2025-04-08 11:56:39</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
     </row>
@@ -565,19 +565,11 @@
       <c r="C6" t="n">
         <v>300</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Milica1</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>2025-04-06 22:18:50</t>
-        </is>
-      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
     </row>
@@ -613,19 +605,11 @@
       <c r="C8" t="n">
         <v>300</v>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Milica1</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>2025-04-06 22:19:14</t>
-        </is>
-      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
     </row>
@@ -641,19 +625,11 @@
       <c r="C9" t="n">
         <v>300</v>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Milica1</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>2025-04-06 22:18:50</t>
-        </is>
-      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
     </row>
@@ -689,11 +665,19 @@
       <c r="C11" t="n">
         <v>300</v>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Milica1</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2025-04-08 11:56:40</t>
+        </is>
+      </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
     </row>
@@ -714,28 +698,6 @@
       <c r="F12" t="inlineStr">
         <is>
           <t>False</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="n">
-        <v>26002680638</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Milica1</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>2025-04-06 22:18:57</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>True</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Serbian language output fixes
</commit_message>
<xml_diff>
--- a/backend/reports/scanned_boxes_report.xlsx
+++ b/backend/reports/scanned_boxes_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,32 +436,32 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>client</t>
+          <t>Klijent</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>box</t>
+          <t>Kutija</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>batch</t>
+          <t>Tura</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>scanned_by</t>
+          <t>Skenirao</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>scan_time</t>
+          <t>Vreme skeniranja</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>present</t>
+          <t>Nalazila se u bazi</t>
         </is>
       </c>
     </row>
@@ -484,11 +484,13 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-04-09 13:06:41</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
+          <t>2025-04-09 14:08:54</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -510,11 +512,13 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-04-09 13:07:16</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>1</v>
+          <t>2025-04-09 14:08:58</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -536,11 +540,13 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-04-09 13:07:17</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
+          <t>2025-04-09 14:08:56</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -562,11 +568,13 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-04-09 13:07:15</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>1</v>
+          <t>2025-04-09 14:09:00</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -588,11 +596,13 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-04-09 13:07:19</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>1</v>
+          <t>2025-04-09 14:09:32</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -614,11 +624,13 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-04-09 13:07:20</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>1</v>
+          <t>2025-04-09 14:09:01</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -640,11 +652,13 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-04-09 13:07:21</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>1</v>
+          <t>2025-04-09 14:09:37</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -666,11 +680,13 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-04-09 13:07:23</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>1</v>
+          <t>2025-04-09 14:09:49</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -692,11 +708,13 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-04-09 13:07:24</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>1</v>
+          <t>2025-04-09 14:09:35</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -718,11 +736,13 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-04-09 13:07:27</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
-        <v>1</v>
+          <t>2025-04-09 14:09:39</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -744,17 +764,19 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-04-09 13:07:28</t>
-        </is>
-      </c>
-      <c r="F12" t="n">
-        <v>1</v>
+          <t>2025-04-09 14:09:50</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
       <c r="B13" t="n">
-        <v>26002680642</v>
+        <v>26002680643</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
@@ -764,11 +786,35 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-04-09 13:06:52</t>
-        </is>
-      </c>
-      <c r="F13" t="n">
-        <v>0</v>
+          <t>2025-04-09 14:09:06</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="n">
+        <v>26002680641</v>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Milica1</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2025-04-09 14:09:53</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finally added report after finishing scan
</commit_message>
<xml_diff>
--- a/backend/reports/scanned_boxes_report.xlsx
+++ b/backend/reports/scanned_boxes_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,7 +484,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-04-09 21:47:21</t>
+          <t>2025-04-10 18:27:32</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -512,7 +512,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-04-09 21:47:29</t>
+          <t>2025-04-10 18:27:32</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -540,7 +540,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-04-09 22:59:28</t>
+          <t>2025-04-10 18:27:34</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -568,7 +568,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-04-09 22:59:37</t>
+          <t>2025-04-10 18:27:29</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -596,7 +596,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-04-09 21:47:23</t>
+          <t>2025-04-10 18:27:29</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -624,7 +624,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-04-09 21:47:26</t>
+          <t>2025-04-10 18:27:33</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -652,7 +652,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-04-09 23:05:25</t>
+          <t>2025-04-10 18:27:28</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -680,7 +680,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-04-09 23:03:42</t>
+          <t>2025-04-10 18:27:27</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -708,7 +708,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-04-09 22:59:35</t>
+          <t>2025-04-10 18:27:34</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -736,7 +736,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-04-09 22:59:43</t>
+          <t>2025-04-10 18:27:35</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -764,78 +764,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-04-09 23:03:46</t>
+          <t>2025-04-10 18:27:36</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
           <t>True</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="n">
-        <v>26002680640</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Milica1</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>2025-04-09 22:58:57</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr"/>
-      <c r="B14" t="n">
-        <v>26002680638</v>
-      </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Milica1</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>2025-04-09 22:59:41</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr"/>
-      <c r="B15" t="n">
-        <v>26002680646</v>
-      </c>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Milica1</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>2025-04-09 23:04:09</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>False</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Error sound on wrong scan and gui changes
</commit_message>
<xml_diff>
--- a/backend/reports/scanned_boxes_report.xlsx
+++ b/backend/reports/scanned_boxes_report.xlsx
@@ -484,7 +484,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-04-10 19:06:15</t>
+          <t>2025-04-11 13:21:07</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -512,7 +512,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-04-10 19:06:17</t>
+          <t>2025-04-11 13:21:11</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -540,7 +540,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-04-10 19:06:18</t>
+          <t>2025-04-11 13:21:14</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -568,7 +568,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-04-10 19:06:40</t>
+          <t>2025-04-11 13:21:38</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -596,7 +596,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-04-10 19:06:20</t>
+          <t>2025-04-11 13:21:39</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -624,7 +624,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-04-10 19:06:37</t>
+          <t>2025-04-11 13:21:43</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -652,7 +652,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-04-10 19:06:54</t>
+          <t>2025-04-11 13:21:51</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -680,7 +680,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-04-10 19:06:43</t>
+          <t>2025-04-11 13:21:49</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -708,7 +708,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-04-10 19:06:21</t>
+          <t>2025-04-11 13:21:46</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -736,7 +736,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-04-10 19:06:42</t>
+          <t>2025-04-11 13:21:46</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -764,7 +764,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-04-10 19:07:12</t>
+          <t>2025-04-11 13:21:47</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -776,7 +776,7 @@
     <row r="13">
       <c r="A13" t="inlineStr"/>
       <c r="B13" t="n">
-        <v>26002680646</v>
+        <v>26002680643</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
@@ -786,7 +786,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-04-10 19:06:22</t>
+          <t>2025-04-11 13:21:23</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">

</xml_diff>

<commit_message>
Small fixes and changes
</commit_message>
<xml_diff>
--- a/backend/reports/scanned_boxes_report.xlsx
+++ b/backend/reports/scanned_boxes_report.xlsx
@@ -484,7 +484,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-04-11 13:21:07</t>
+          <t>2025-04-14 19:42:47</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -512,7 +512,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-04-11 13:21:11</t>
+          <t>2025-04-14 19:42:46</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -540,7 +540,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-04-11 13:21:14</t>
+          <t>2025-04-14 19:42:47</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -568,7 +568,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-04-11 13:21:38</t>
+          <t>2025-04-14 19:42:49</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -596,7 +596,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-04-11 13:21:39</t>
+          <t>2025-04-14 19:42:51</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -624,7 +624,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-04-11 13:21:43</t>
+          <t>2025-04-14 19:42:53</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -652,7 +652,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-04-11 13:21:51</t>
+          <t>2025-04-14 19:42:54</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -680,7 +680,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-04-11 13:21:49</t>
+          <t>2025-04-14 19:42:55</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -708,7 +708,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-04-11 13:21:46</t>
+          <t>2025-04-14 19:42:55</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -736,7 +736,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-04-11 13:21:46</t>
+          <t>2025-04-14 19:42:57</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -764,7 +764,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-04-11 13:21:47</t>
+          <t>2025-04-14 19:42:58</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -776,7 +776,7 @@
     <row r="13">
       <c r="A13" t="inlineStr"/>
       <c r="B13" t="n">
-        <v>26002680643</v>
+        <v>26002680638</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
@@ -786,7 +786,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-04-11 13:21:23</t>
+          <t>2025-04-14 19:42:59</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">

</xml_diff>